<commit_message>
Description of your changes
</commit_message>
<xml_diff>
--- a/Class Cancellation App.xlsx
+++ b/Class Cancellation App.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rebecca\Class Cancellation app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C1140A-1CE7-47F3-B3AC-EA387BAF9F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F3D269-0FD4-43FD-AAD0-0C6C8BF8706C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,13 @@
     <sheet name="Saturday" sheetId="14" r:id="rId6"/>
     <sheet name="Additions" sheetId="15" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Friday!$A$1:$N$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monday!$A$1:$N$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Thursday!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tuesday!$A$1:$N$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Wednesday!$A$1:$N$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2986" uniqueCount="937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1086">
   <si>
     <t>Date</t>
   </si>
@@ -2850,6 +2857,453 @@
   </si>
   <si>
     <t>01:30 AM - 02:00 AM</t>
+  </si>
+  <si>
+    <t>Credits have been issued</t>
+  </si>
+  <si>
+    <t>00027649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$42.93 </t>
+  </si>
+  <si>
+    <t>00028354</t>
+  </si>
+  <si>
+    <t>00028373</t>
+  </si>
+  <si>
+    <t>00028434</t>
+  </si>
+  <si>
+    <t>Pickleball Skills &amp; Drills Intro</t>
+  </si>
+  <si>
+    <t>00028372</t>
+  </si>
+  <si>
+    <t>Pickleball Skills &amp; Drills Social Beginner</t>
+  </si>
+  <si>
+    <t>Tim Salmon</t>
+  </si>
+  <si>
+    <t>00027698</t>
+  </si>
+  <si>
+    <t>Laura Garofalo</t>
+  </si>
+  <si>
+    <t>00027997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$30.33 </t>
+  </si>
+  <si>
+    <t>00028553</t>
+  </si>
+  <si>
+    <t>00027739</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$45.04 </t>
+  </si>
+  <si>
+    <t>00027913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$43.06 </t>
+  </si>
+  <si>
+    <t>09:00 AM - 10:10 AM</t>
+  </si>
+  <si>
+    <t>00028724</t>
+  </si>
+  <si>
+    <t>00028306</t>
+  </si>
+  <si>
+    <t>Woodcarving Rendezvous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$35.55 </t>
+  </si>
+  <si>
+    <t>Mark Sheridan</t>
+  </si>
+  <si>
+    <t>SCL - Seniors Centre Loyalist Odessa</t>
+  </si>
+  <si>
+    <t>00027639</t>
+  </si>
+  <si>
+    <t>Line Dancing Improver Continued</t>
+  </si>
+  <si>
+    <t>00027813</t>
+  </si>
+  <si>
+    <t>Spanish Intermediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$96.30 </t>
+  </si>
+  <si>
+    <t>00027668</t>
+  </si>
+  <si>
+    <t>00027675</t>
+  </si>
+  <si>
+    <t>00028725</t>
+  </si>
+  <si>
+    <t>00027803</t>
+  </si>
+  <si>
+    <t>Italian Intermediate Continued</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$86.08 </t>
+  </si>
+  <si>
+    <t>00028262</t>
+  </si>
+  <si>
+    <t>Painting Without a Brush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$153.36 </t>
+  </si>
+  <si>
+    <t>10:00 AM - 12:30 PM</t>
+  </si>
+  <si>
+    <t>00028549</t>
+  </si>
+  <si>
+    <t>Step Fit</t>
+  </si>
+  <si>
+    <t>00027762</t>
+  </si>
+  <si>
+    <t>Tai Chi Beginner</t>
+  </si>
+  <si>
+    <t>00027868</t>
+  </si>
+  <si>
+    <t>Ballroom &amp; Latin Dance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$39.24 </t>
+  </si>
+  <si>
+    <t>Dave Almas</t>
+  </si>
+  <si>
+    <t>00027638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$48.42 </t>
+  </si>
+  <si>
+    <t>00028375</t>
+  </si>
+  <si>
+    <t>Mon 08/09/2025 - Tue 11/11/2025</t>
+  </si>
+  <si>
+    <t>00027663</t>
+  </si>
+  <si>
+    <t>Marion McCabe</t>
+  </si>
+  <si>
+    <t>00028358</t>
+  </si>
+  <si>
+    <t>Gail Beck</t>
+  </si>
+  <si>
+    <t>00027645</t>
+  </si>
+  <si>
+    <t>Judy Kay</t>
+  </si>
+  <si>
+    <t>00027923</t>
+  </si>
+  <si>
+    <t>10:30 AM - 11:40 AM</t>
+  </si>
+  <si>
+    <t>00027811</t>
+  </si>
+  <si>
+    <t>Spanish Intermediate Continued</t>
+  </si>
+  <si>
+    <t>11:15 AM - 12:45 PM</t>
+  </si>
+  <si>
+    <t>00027763</t>
+  </si>
+  <si>
+    <t>Essentrics®</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$74.34 </t>
+  </si>
+  <si>
+    <t>00028241</t>
+  </si>
+  <si>
+    <t>Guitar &amp; Uke Rendezvous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$59.13 </t>
+  </si>
+  <si>
+    <t>00028564</t>
+  </si>
+  <si>
+    <t>Crocheting &amp; Knitting Rendezvous</t>
+  </si>
+  <si>
+    <t>12:00 PM - 01:30 PM</t>
+  </si>
+  <si>
+    <t>00027637</t>
+  </si>
+  <si>
+    <t>00027798</t>
+  </si>
+  <si>
+    <t>Dance For Parkinson's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$66.08 </t>
+  </si>
+  <si>
+    <t>Amy Booth</t>
+  </si>
+  <si>
+    <t>00028368</t>
+  </si>
+  <si>
+    <t>Karen Greene</t>
+  </si>
+  <si>
+    <t>00028360</t>
+  </si>
+  <si>
+    <t>00027778</t>
+  </si>
+  <si>
+    <t>Hot Topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$32.40 </t>
+  </si>
+  <si>
+    <t>Ron Turley</t>
+  </si>
+  <si>
+    <t>00027640</t>
+  </si>
+  <si>
+    <t>00027898</t>
+  </si>
+  <si>
+    <t>Scrabble Rendezvous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$34.11 </t>
+  </si>
+  <si>
+    <t>Paul Kennedy</t>
+  </si>
+  <si>
+    <t>00028349</t>
+  </si>
+  <si>
+    <t>Sculpture</t>
+  </si>
+  <si>
+    <t>00028305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$32.94 </t>
+  </si>
+  <si>
+    <t>00027818</t>
+  </si>
+  <si>
+    <t>Watercolour Beginner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$160.96 </t>
+  </si>
+  <si>
+    <t>00027870</t>
+  </si>
+  <si>
+    <t>01:15 PM - 02:45 PM</t>
+  </si>
+  <si>
+    <t>00027764</t>
+  </si>
+  <si>
+    <t>Jam Session</t>
+  </si>
+  <si>
+    <t>01:30 PM - 04:00 PM</t>
+  </si>
+  <si>
+    <t>00028246</t>
+  </si>
+  <si>
+    <t>Stamps &amp; Their Stories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$38.88 </t>
+  </si>
+  <si>
+    <t>Hugh MacDonald</t>
+  </si>
+  <si>
+    <t>00027924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$26.46 </t>
+  </si>
+  <si>
+    <t>00027648</t>
+  </si>
+  <si>
+    <t>Trending Topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$36.09 </t>
+  </si>
+  <si>
+    <t>John Fleischmann</t>
+  </si>
+  <si>
+    <t>00027804</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$82.17 </t>
+  </si>
+  <si>
+    <t>Craig Edwards</t>
+  </si>
+  <si>
+    <t>02:00 PM - 03:30 PM</t>
+  </si>
+  <si>
+    <t>00027642</t>
+  </si>
+  <si>
+    <t>Public Speaking</t>
+  </si>
+  <si>
+    <t>Brian Sutton</t>
+  </si>
+  <si>
+    <t>00028362</t>
+  </si>
+  <si>
+    <t>00028706</t>
+  </si>
+  <si>
+    <t>00027767</t>
+  </si>
+  <si>
+    <t>Coffee House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$93.33 </t>
+  </si>
+  <si>
+    <t>Michael George</t>
+  </si>
+  <si>
+    <t>04:30 PM - 06:30 PM</t>
+  </si>
+  <si>
+    <t>00028011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$69.66 </t>
+  </si>
+  <si>
+    <t>00027998</t>
+  </si>
+  <si>
+    <t>Wendy Mitchell</t>
+  </si>
+  <si>
+    <t>00027911</t>
+  </si>
+  <si>
+    <t>Jean Barkley</t>
+  </si>
+  <si>
+    <t>00028304</t>
+  </si>
+  <si>
+    <t>Mon 15/09/2025 - Mon 10/11/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$38.24 </t>
+  </si>
+  <si>
+    <t>00028696</t>
+  </si>
+  <si>
+    <t>Mon 15/09/2025</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Avoiding Scams &amp; Protecting Your Identity</t>
+  </si>
+  <si>
+    <t>00028697</t>
+  </si>
+  <si>
+    <t>Mon 22/09/2025</t>
+  </si>
+  <si>
+    <t>How the Internet Works</t>
+  </si>
+  <si>
+    <t>12:00 AM - 01:00 AM</t>
+  </si>
+  <si>
+    <t>00028698</t>
+  </si>
+  <si>
+    <t>Mon 29/09/2025</t>
+  </si>
+  <si>
+    <t>Selecting a Smart Phone</t>
+  </si>
+  <si>
+    <t>Oct 3, 2025;  Oct 10, 2025; Oct 17, 2025</t>
+  </si>
+  <si>
+    <t>Oct 7, 2025; Oct 14, 2025; Oct 21, 2025</t>
+  </si>
+  <si>
+    <t>Oct 7. 2025; Oct 14, 2025; Oct 21, 2025</t>
   </si>
 </sst>
 </file>
@@ -2897,10 +3351,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3205,10 +3660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772A3901-ADF4-4CA6-84A1-B1B329A6EAAE}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3216,12 +3671,12 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
@@ -3274,34 +3729,31 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>119</v>
+        <v>250</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>251</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>252</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>124</v>
+        <v>253</v>
       </c>
       <c r="H2" t="s">
-        <v>125</v>
+        <v>254</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="J2" t="s">
         <v>126</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
       <c r="L2" t="b">
         <v>0</v>
@@ -3309,25 +3761,25 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>127</v>
+        <v>676</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>677</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>678</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>494</v>
       </c>
       <c r="G3" t="s">
-        <v>124</v>
+        <v>679</v>
       </c>
       <c r="H3" t="s">
-        <v>130</v>
+        <v>496</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -3336,7 +3788,7 @@
         <v>126</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="L3" t="b">
         <v>0</v>
@@ -3344,34 +3796,34 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>131</v>
+        <v>737</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>677</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>678</v>
       </c>
       <c r="F4" t="s">
-        <v>123</v>
+        <v>494</v>
       </c>
       <c r="G4" t="s">
-        <v>124</v>
+        <v>679</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>738</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="J4" t="s">
         <v>126</v>
       </c>
       <c r="K4" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="L4" t="b">
         <v>0</v>
@@ -3379,34 +3831,34 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>133</v>
+        <v>938</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>172</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
+        <v>229</v>
       </c>
       <c r="G5" t="s">
-        <v>124</v>
+        <v>939</v>
       </c>
       <c r="H5" t="s">
-        <v>125</v>
+        <v>254</v>
       </c>
       <c r="I5" t="s">
-        <v>135</v>
+        <v>7</v>
       </c>
       <c r="J5" t="s">
         <v>126</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>255</v>
       </c>
       <c r="L5" t="b">
         <v>0</v>
@@ -3414,34 +3866,31 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>136</v>
+        <v>940</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>172</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>123</v>
+        <v>534</v>
       </c>
       <c r="G6" t="s">
-        <v>124</v>
+        <v>592</v>
       </c>
       <c r="H6" t="s">
-        <v>137</v>
+        <v>499</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>500</v>
       </c>
       <c r="J6" t="s">
         <v>126</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="L6" t="b">
         <v>0</v>
@@ -3449,34 +3898,31 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>138</v>
+        <v>941</v>
       </c>
       <c r="C7" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>141</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>142</v>
+        <v>592</v>
       </c>
       <c r="H7" t="s">
-        <v>143</v>
+        <v>499</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>500</v>
       </c>
       <c r="J7" t="s">
         <v>126</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
@@ -3484,25 +3930,25 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>144</v>
+        <v>942</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>943</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>323</v>
       </c>
       <c r="G8" t="s">
-        <v>146</v>
+        <v>614</v>
       </c>
       <c r="H8" t="s">
-        <v>147</v>
+        <v>659</v>
       </c>
       <c r="I8" t="s">
         <v>13</v>
@@ -3511,7 +3957,7 @@
         <v>126</v>
       </c>
       <c r="K8" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="L8" t="b">
         <v>0</v>
@@ -3519,34 +3965,31 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>148</v>
+        <v>944</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>149</v>
+        <v>945</v>
       </c>
       <c r="G9" t="s">
-        <v>150</v>
+        <v>614</v>
       </c>
       <c r="H9" t="s">
-        <v>151</v>
+        <v>946</v>
       </c>
       <c r="I9" t="s">
-        <v>7</v>
+        <v>500</v>
       </c>
       <c r="J9" t="s">
         <v>126</v>
       </c>
       <c r="K9" t="s">
-        <v>152</v>
+        <v>11</v>
       </c>
       <c r="L9" t="b">
         <v>0</v>
@@ -3554,34 +3997,34 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>153</v>
+        <v>947</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>261</v>
       </c>
       <c r="F10" t="s">
-        <v>149</v>
+        <v>262</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>948</v>
       </c>
       <c r="I10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J10" t="s">
         <v>126</v>
       </c>
       <c r="K10" t="s">
-        <v>31</v>
+        <v>265</v>
       </c>
       <c r="L10" t="b">
         <v>0</v>
@@ -3589,31 +4032,34 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>154</v>
+        <v>949</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>219</v>
       </c>
       <c r="G11" t="s">
-        <v>150</v>
+        <v>950</v>
       </c>
       <c r="H11" t="s">
-        <v>151</v>
+        <v>427</v>
       </c>
       <c r="I11" t="s">
-        <v>6</v>
+        <v>176</v>
       </c>
       <c r="J11" t="s">
         <v>126</v>
       </c>
       <c r="K11" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="L11" t="b">
         <v>0</v>
@@ -3621,34 +4067,34 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>155</v>
+        <v>951</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>428</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
+        <v>363</v>
       </c>
       <c r="G12" t="s">
-        <v>150</v>
+        <v>429</v>
       </c>
       <c r="H12" t="s">
-        <v>125</v>
+        <v>430</v>
       </c>
       <c r="I12" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s">
         <v>126</v>
       </c>
       <c r="K12" t="s">
-        <v>156</v>
+        <v>17</v>
       </c>
       <c r="L12" t="b">
         <v>0</v>
@@ -3656,25 +4102,25 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>157</v>
+        <v>952</v>
       </c>
       <c r="C13" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="D13" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>870</v>
       </c>
       <c r="F13" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="G13" t="s">
-        <v>150</v>
+        <v>953</v>
       </c>
       <c r="H13" t="s">
-        <v>161</v>
+        <v>436</v>
       </c>
       <c r="I13" t="s">
         <v>7</v>
@@ -3691,25 +4137,25 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>162</v>
+        <v>954</v>
       </c>
       <c r="C14" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="D14" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
+        <v>955</v>
       </c>
       <c r="H14" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="I14" t="s">
         <v>7</v>
@@ -3718,7 +4164,7 @@
         <v>126</v>
       </c>
       <c r="K14" t="s">
-        <v>55</v>
+        <v>956</v>
       </c>
       <c r="L14" t="b">
         <v>0</v>
@@ -3726,34 +4172,34 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>164</v>
+        <v>957</v>
       </c>
       <c r="C15" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>713</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>431</v>
       </c>
       <c r="G15" t="s">
-        <v>150</v>
+        <v>429</v>
       </c>
       <c r="H15" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="I15" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="J15" t="s">
         <v>126</v>
       </c>
       <c r="K15" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="L15" t="b">
         <v>0</v>
@@ -3761,34 +4207,31 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>165</v>
+        <v>958</v>
       </c>
       <c r="C16" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="D16" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="E16" t="s">
-        <v>128</v>
-      </c>
-      <c r="F16" t="s">
-        <v>166</v>
+        <v>959</v>
       </c>
       <c r="G16" t="s">
-        <v>150</v>
+        <v>960</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>961</v>
       </c>
       <c r="I16" t="s">
-        <v>167</v>
+        <v>962</v>
       </c>
       <c r="J16" t="s">
         <v>126</v>
       </c>
       <c r="K16" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="L16" t="b">
         <v>0</v>
@@ -3796,42 +4239,42 @@
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>168</v>
+        <v>963</v>
       </c>
       <c r="C17" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>964</v>
       </c>
       <c r="F17" t="s">
-        <v>129</v>
+        <v>174</v>
       </c>
       <c r="G17" t="s">
-        <v>150</v>
+        <v>244</v>
       </c>
       <c r="H17" t="s">
-        <v>137</v>
+        <v>666</v>
       </c>
       <c r="I17" t="s">
-        <v>7</v>
+        <v>135</v>
       </c>
       <c r="J17" t="s">
         <v>126</v>
       </c>
       <c r="K17" t="s">
-        <v>29</v>
+        <v>681</v>
       </c>
       <c r="L17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>171</v>
+        <v>965</v>
       </c>
       <c r="C18" t="s">
         <v>172</v>
@@ -3840,25 +4283,25 @@
         <v>173</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>966</v>
       </c>
       <c r="F18" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G18" t="s">
-        <v>175</v>
+        <v>967</v>
       </c>
       <c r="H18" t="s">
-        <v>125</v>
+        <v>514</v>
       </c>
       <c r="I18" t="s">
-        <v>176</v>
+        <v>7</v>
       </c>
       <c r="J18" t="s">
         <v>126</v>
       </c>
       <c r="K18" t="s">
-        <v>21</v>
+        <v>598</v>
       </c>
       <c r="L18" t="b">
         <v>0</v>
@@ -3866,7 +4309,7 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>177</v>
+        <v>968</v>
       </c>
       <c r="C19" t="s">
         <v>172</v>
@@ -3875,25 +4318,25 @@
         <v>173</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>261</v>
       </c>
       <c r="F19" t="s">
-        <v>149</v>
+        <v>262</v>
       </c>
       <c r="G19" t="s">
-        <v>175</v>
+        <v>400</v>
       </c>
       <c r="H19" t="s">
-        <v>125</v>
+        <v>948</v>
       </c>
       <c r="I19" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J19" t="s">
         <v>126</v>
       </c>
       <c r="K19" t="s">
-        <v>31</v>
+        <v>279</v>
       </c>
       <c r="L19" t="b">
         <v>0</v>
@@ -3901,22 +4344,22 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>178</v>
+        <v>969</v>
       </c>
       <c r="C20" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F20" t="s">
         <v>141</v>
       </c>
       <c r="G20" t="s">
-        <v>180</v>
+        <v>244</v>
       </c>
       <c r="H20" t="s">
         <v>147</v>
@@ -3928,48 +4371,1606 @@
         <v>126</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="L20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>181</v>
+        <v>970</v>
       </c>
       <c r="C21" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
         <v>173</v>
       </c>
       <c r="E21" t="s">
+        <v>428</v>
+      </c>
+      <c r="F21" t="s">
+        <v>431</v>
+      </c>
+      <c r="G21" t="s">
+        <v>429</v>
+      </c>
+      <c r="H21" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" t="s">
+        <v>126</v>
+      </c>
+      <c r="K21" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>971</v>
+      </c>
+      <c r="C22" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" t="s">
+        <v>972</v>
+      </c>
+      <c r="F22" t="s">
+        <v>305</v>
+      </c>
+      <c r="G22" t="s">
+        <v>973</v>
+      </c>
+      <c r="H22" t="s">
+        <v>804</v>
+      </c>
+      <c r="I22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" t="s">
+        <v>126</v>
+      </c>
+      <c r="K22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>974</v>
+      </c>
+      <c r="C23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" t="s">
+        <v>975</v>
+      </c>
+      <c r="F23" t="s">
+        <v>134</v>
+      </c>
+      <c r="G23" t="s">
+        <v>976</v>
+      </c>
+      <c r="H23" t="s">
+        <v>327</v>
+      </c>
+      <c r="I23" t="s">
+        <v>176</v>
+      </c>
+      <c r="J23" t="s">
+        <v>126</v>
+      </c>
+      <c r="K23" t="s">
+        <v>977</v>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" t="s">
+        <v>174</v>
+      </c>
+      <c r="G24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H24" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" t="s">
+        <v>176</v>
+      </c>
+      <c r="J24" t="s">
+        <v>126</v>
+      </c>
+      <c r="K24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>978</v>
+      </c>
+      <c r="C25" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" t="s">
+        <v>173</v>
+      </c>
+      <c r="E25" t="s">
+        <v>979</v>
+      </c>
+      <c r="F25" t="s">
+        <v>363</v>
+      </c>
+      <c r="G25" t="s">
+        <v>244</v>
+      </c>
+      <c r="H25" t="s">
+        <v>430</v>
+      </c>
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" t="s">
+        <v>126</v>
+      </c>
+      <c r="K25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>980</v>
+      </c>
+      <c r="C26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" t="s">
+        <v>981</v>
+      </c>
+      <c r="F26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G26" t="s">
+        <v>617</v>
+      </c>
+      <c r="H26" t="s">
+        <v>618</v>
+      </c>
+      <c r="I26" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" t="s">
+        <v>126</v>
+      </c>
+      <c r="K26" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>982</v>
+      </c>
+      <c r="C27" t="s">
+        <v>172</v>
+      </c>
+      <c r="D27" t="s">
+        <v>173</v>
+      </c>
+      <c r="E27" t="s">
+        <v>983</v>
+      </c>
+      <c r="F27" t="s">
+        <v>183</v>
+      </c>
+      <c r="G27" t="s">
+        <v>984</v>
+      </c>
+      <c r="H27" t="s">
+        <v>985</v>
+      </c>
+      <c r="I27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" t="s">
+        <v>126</v>
+      </c>
+      <c r="K27" t="s">
+        <v>366</v>
+      </c>
+      <c r="L27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>986</v>
+      </c>
+      <c r="C28" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" t="s">
+        <v>174</v>
+      </c>
+      <c r="G28" t="s">
+        <v>987</v>
+      </c>
+      <c r="H28" t="s">
+        <v>506</v>
+      </c>
+      <c r="I28" t="s">
+        <v>135</v>
+      </c>
+      <c r="J28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K28" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>988</v>
+      </c>
+      <c r="C29" t="s">
+        <v>989</v>
+      </c>
+      <c r="D29" t="s">
+        <v>173</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>592</v>
+      </c>
+      <c r="H29" t="s">
+        <v>499</v>
+      </c>
+      <c r="I29" t="s">
+        <v>500</v>
+      </c>
+      <c r="J29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K29" t="s">
+        <v>27</v>
+      </c>
+      <c r="L29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>990</v>
+      </c>
+      <c r="C30" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" t="s">
+        <v>173</v>
+      </c>
+      <c r="E30" t="s">
+        <v>536</v>
+      </c>
+      <c r="F30" t="s">
+        <v>323</v>
+      </c>
+      <c r="G30" t="s">
+        <v>592</v>
+      </c>
+      <c r="H30" t="s">
+        <v>991</v>
+      </c>
+      <c r="I30" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" t="s">
+        <v>126</v>
+      </c>
+      <c r="K30" t="s">
+        <v>27</v>
+      </c>
+      <c r="L30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>992</v>
+      </c>
+      <c r="C31" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" t="s">
+        <v>173</v>
+      </c>
+      <c r="E31" t="s">
+        <v>561</v>
+      </c>
+      <c r="G31" t="s">
+        <v>592</v>
+      </c>
+      <c r="H31" t="s">
+        <v>993</v>
+      </c>
+      <c r="I31" t="s">
+        <v>500</v>
+      </c>
+      <c r="J31" t="s">
+        <v>126</v>
+      </c>
+      <c r="K31" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>994</v>
+      </c>
+      <c r="C32" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" t="s">
+        <v>289</v>
+      </c>
+      <c r="G32" t="s">
+        <v>526</v>
+      </c>
+      <c r="H32" t="s">
+        <v>995</v>
+      </c>
+      <c r="I32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" t="s">
+        <v>126</v>
+      </c>
+      <c r="K32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>996</v>
+      </c>
+      <c r="C33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" t="s">
+        <v>955</v>
+      </c>
+      <c r="H33" t="s">
+        <v>125</v>
+      </c>
+      <c r="I33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" t="s">
+        <v>126</v>
+      </c>
+      <c r="K33" t="s">
+        <v>997</v>
+      </c>
+      <c r="L33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>998</v>
+      </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" t="s">
+        <v>173</v>
+      </c>
+      <c r="E34" t="s">
+        <v>999</v>
+      </c>
+      <c r="F34" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" t="s">
+        <v>967</v>
+      </c>
+      <c r="H34" t="s">
+        <v>514</v>
+      </c>
+      <c r="I34" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" t="s">
+        <v>126</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1000</v>
+      </c>
+      <c r="L34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C35" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1002</v>
+      </c>
+      <c r="F35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H35" t="s">
+        <v>333</v>
+      </c>
+      <c r="I35" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" t="s">
+        <v>126</v>
+      </c>
+      <c r="K35" t="s">
+        <v>29</v>
+      </c>
+      <c r="L35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C36" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" t="s">
+        <v>173</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F36" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H36" t="s">
+        <v>273</v>
+      </c>
+      <c r="I36" t="s">
+        <v>176</v>
+      </c>
+      <c r="J36" t="s">
+        <v>126</v>
+      </c>
+      <c r="K36" t="s">
+        <v>213</v>
+      </c>
+      <c r="L36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>1007</v>
+      </c>
+      <c r="C37" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1008</v>
+      </c>
+      <c r="F37" t="s">
+        <v>174</v>
+      </c>
+      <c r="G37" t="s">
+        <v>244</v>
+      </c>
+      <c r="H37" t="s">
+        <v>161</v>
+      </c>
+      <c r="I37" t="s">
+        <v>135</v>
+      </c>
+      <c r="J37" t="s">
+        <v>126</v>
+      </c>
+      <c r="K37" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C38" t="s">
+        <v>172</v>
+      </c>
+      <c r="D38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" t="s">
+        <v>174</v>
+      </c>
+      <c r="G38" t="s">
+        <v>244</v>
+      </c>
+      <c r="H38" t="s">
+        <v>147</v>
+      </c>
+      <c r="I38" t="s">
+        <v>135</v>
+      </c>
+      <c r="J38" t="s">
+        <v>126</v>
+      </c>
+      <c r="K38" t="s">
+        <v>31</v>
+      </c>
+      <c r="L38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" t="s">
+        <v>173</v>
+      </c>
+      <c r="E39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" t="s">
+        <v>149</v>
+      </c>
+      <c r="G39" t="s">
+        <v>175</v>
+      </c>
+      <c r="H39" t="s">
+        <v>125</v>
+      </c>
+      <c r="I39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" t="s">
+        <v>126</v>
+      </c>
+      <c r="K39" t="s">
+        <v>31</v>
+      </c>
+      <c r="L39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>1011</v>
+      </c>
+      <c r="C40" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F40" t="s">
+        <v>305</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H40" t="s">
+        <v>1014</v>
+      </c>
+      <c r="I40" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" t="s">
+        <v>126</v>
+      </c>
+      <c r="K40" t="s">
+        <v>32</v>
+      </c>
+      <c r="L40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C41" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" t="s">
+        <v>173</v>
+      </c>
+      <c r="E41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G41" t="s">
+        <v>592</v>
+      </c>
+      <c r="H41" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I41" t="s">
+        <v>500</v>
+      </c>
+      <c r="J41" t="s">
+        <v>126</v>
+      </c>
+      <c r="K41" t="s">
+        <v>34</v>
+      </c>
+      <c r="L41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>1017</v>
+      </c>
+      <c r="C42" t="s">
+        <v>172</v>
+      </c>
+      <c r="D42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" t="s">
+        <v>592</v>
+      </c>
+      <c r="H42" t="s">
+        <v>1016</v>
+      </c>
+      <c r="I42" t="s">
+        <v>500</v>
+      </c>
+      <c r="J42" t="s">
+        <v>126</v>
+      </c>
+      <c r="K42" t="s">
+        <v>34</v>
+      </c>
+      <c r="L42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C43" t="s">
+        <v>172</v>
+      </c>
+      <c r="D43" t="s">
+        <v>173</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F43" t="s">
+        <v>134</v>
+      </c>
+      <c r="G43" t="s">
+        <v>1020</v>
+      </c>
+      <c r="H43" t="s">
+        <v>1021</v>
+      </c>
+      <c r="I43" t="s">
+        <v>135</v>
+      </c>
+      <c r="J43" t="s">
+        <v>126</v>
+      </c>
+      <c r="K43" t="s">
+        <v>37</v>
+      </c>
+      <c r="L43" t="b">
+        <v>0</v>
+      </c>
+      <c r="M43" s="3">
+        <v>45971</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" t="s">
+        <v>173</v>
+      </c>
+      <c r="E44" t="s">
+        <v>571</v>
+      </c>
+      <c r="F44" t="s">
+        <v>174</v>
+      </c>
+      <c r="G44" t="s">
+        <v>244</v>
+      </c>
+      <c r="H44" t="s">
+        <v>147</v>
+      </c>
+      <c r="I44" t="s">
+        <v>135</v>
+      </c>
+      <c r="J44" t="s">
+        <v>126</v>
+      </c>
+      <c r="K44" t="s">
+        <v>37</v>
+      </c>
+      <c r="L44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C45" t="s">
+        <v>172</v>
+      </c>
+      <c r="D45" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F45" t="s">
+        <v>193</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H45" t="s">
+        <v>1026</v>
+      </c>
+      <c r="I45" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45" t="s">
+        <v>126</v>
+      </c>
+      <c r="K45" t="s">
+        <v>9</v>
+      </c>
+      <c r="L45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C46" t="s">
+        <v>172</v>
+      </c>
+      <c r="D46" t="s">
+        <v>173</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F46" t="s">
+        <v>134</v>
+      </c>
+      <c r="G46" t="s">
+        <v>244</v>
+      </c>
+      <c r="H46" t="s">
+        <v>723</v>
+      </c>
+      <c r="I46" t="s">
+        <v>176</v>
+      </c>
+      <c r="J46" t="s">
+        <v>126</v>
+      </c>
+      <c r="K46" t="s">
+        <v>36</v>
+      </c>
+      <c r="L46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C47" t="s">
+        <v>172</v>
+      </c>
+      <c r="D47" t="s">
+        <v>173</v>
+      </c>
+      <c r="E47" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H47" t="s">
+        <v>125</v>
+      </c>
+      <c r="I47" t="s">
+        <v>962</v>
+      </c>
+      <c r="J47" t="s">
+        <v>126</v>
+      </c>
+      <c r="K47" t="s">
+        <v>36</v>
+      </c>
+      <c r="L47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C48" t="s">
+        <v>172</v>
+      </c>
+      <c r="D48" t="s">
+        <v>173</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F48" t="s">
+        <v>163</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H48" t="s">
+        <v>822</v>
+      </c>
+      <c r="I48" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" t="s">
+        <v>126</v>
+      </c>
+      <c r="K48" t="s">
+        <v>9</v>
+      </c>
+      <c r="L48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C49" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" t="s">
+        <v>173</v>
+      </c>
+      <c r="E49" t="s">
+        <v>56</v>
+      </c>
+      <c r="F49" t="s">
+        <v>160</v>
+      </c>
+      <c r="G49" t="s">
+        <v>967</v>
+      </c>
+      <c r="H49" t="s">
+        <v>514</v>
+      </c>
+      <c r="I49" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" t="s">
+        <v>126</v>
+      </c>
+      <c r="K49" t="s">
+        <v>1035</v>
+      </c>
+      <c r="L49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C50" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" t="s">
+        <v>173</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F50" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" t="s">
+        <v>871</v>
+      </c>
+      <c r="H50" t="s">
+        <v>756</v>
+      </c>
+      <c r="I50" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" t="s">
+        <v>126</v>
+      </c>
+      <c r="K50" t="s">
+        <v>1038</v>
+      </c>
+      <c r="L50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C51" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" t="s">
+        <v>173</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F51" t="s">
+        <v>174</v>
+      </c>
+      <c r="G51" t="s">
+        <v>1041</v>
+      </c>
+      <c r="H51" t="s">
+        <v>1042</v>
+      </c>
+      <c r="I51" t="s">
+        <v>176</v>
+      </c>
+      <c r="J51" t="s">
+        <v>126</v>
+      </c>
+      <c r="K51" t="s">
+        <v>468</v>
+      </c>
+      <c r="L51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C52" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" t="s">
+        <v>173</v>
+      </c>
+      <c r="E52" t="s">
+        <v>39</v>
+      </c>
+      <c r="F52" t="s">
+        <v>149</v>
+      </c>
+      <c r="G52" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H52" t="s">
+        <v>125</v>
+      </c>
+      <c r="I52" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" t="s">
+        <v>126</v>
+      </c>
+      <c r="K52" t="s">
+        <v>40</v>
+      </c>
+      <c r="L52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C53" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" t="s">
+        <v>173</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F53" t="s">
+        <v>229</v>
+      </c>
+      <c r="G53" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H53" t="s">
+        <v>1048</v>
+      </c>
+      <c r="I53" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" t="s">
+        <v>126</v>
+      </c>
+      <c r="K53" t="s">
+        <v>64</v>
+      </c>
+      <c r="L53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C54" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" t="s">
+        <v>173</v>
+      </c>
+      <c r="E54" t="s">
+        <v>108</v>
+      </c>
+      <c r="F54" t="s">
+        <v>305</v>
+      </c>
+      <c r="G54" t="s">
+        <v>1050</v>
+      </c>
+      <c r="H54" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I54" t="s">
+        <v>7</v>
+      </c>
+      <c r="J54" t="s">
+        <v>126</v>
+      </c>
+      <c r="K54" t="s">
+        <v>1052</v>
+      </c>
+      <c r="L54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C55" t="s">
+        <v>172</v>
+      </c>
+      <c r="D55" t="s">
+        <v>173</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1054</v>
+      </c>
+      <c r="F55" t="s">
+        <v>174</v>
+      </c>
+      <c r="G55" t="s">
+        <v>244</v>
+      </c>
+      <c r="H55" t="s">
+        <v>1055</v>
+      </c>
+      <c r="I55" t="s">
+        <v>135</v>
+      </c>
+      <c r="J55" t="s">
+        <v>126</v>
+      </c>
+      <c r="K55" t="s">
+        <v>1052</v>
+      </c>
+      <c r="L55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C56" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" t="s">
+        <v>173</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" t="s">
+        <v>592</v>
+      </c>
+      <c r="H56" t="s">
+        <v>749</v>
+      </c>
+      <c r="I56" t="s">
+        <v>500</v>
+      </c>
+      <c r="J56" t="s">
+        <v>126</v>
+      </c>
+      <c r="K56" t="s">
+        <v>41</v>
+      </c>
+      <c r="L56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C57" t="s">
+        <v>172</v>
+      </c>
+      <c r="D57" t="s">
+        <v>173</v>
+      </c>
+      <c r="E57" t="s">
+        <v>512</v>
+      </c>
+      <c r="F57" t="s">
+        <v>160</v>
+      </c>
+      <c r="G57" t="s">
+        <v>967</v>
+      </c>
+      <c r="H57" t="s">
+        <v>514</v>
+      </c>
+      <c r="I57" t="s">
+        <v>7</v>
+      </c>
+      <c r="J57" t="s">
+        <v>126</v>
+      </c>
+      <c r="K57" t="s">
+        <v>587</v>
+      </c>
+      <c r="L57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C58" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" t="s">
+        <v>173</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F58" t="s">
+        <v>129</v>
+      </c>
+      <c r="G58" t="s">
+        <v>1060</v>
+      </c>
+      <c r="H58" t="s">
+        <v>1061</v>
+      </c>
+      <c r="I58" t="s">
+        <v>7</v>
+      </c>
+      <c r="J58" t="s">
+        <v>126</v>
+      </c>
+      <c r="K58" t="s">
+        <v>1062</v>
+      </c>
+      <c r="L58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C59" t="s">
+        <v>172</v>
+      </c>
+      <c r="D59" t="s">
+        <v>173</v>
+      </c>
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
+        <v>149</v>
+      </c>
+      <c r="G59" t="s">
+        <v>1064</v>
+      </c>
+      <c r="H59" t="s">
+        <v>762</v>
+      </c>
+      <c r="I59" t="s">
+        <v>7</v>
+      </c>
+      <c r="J59" t="s">
+        <v>126</v>
+      </c>
+      <c r="K59" t="s">
+        <v>763</v>
+      </c>
+      <c r="L59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C60" t="s">
+        <v>172</v>
+      </c>
+      <c r="D60" t="s">
+        <v>173</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" t="s">
+        <v>219</v>
+      </c>
+      <c r="G60" t="s">
+        <v>1064</v>
+      </c>
+      <c r="H60" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I60" t="s">
+        <v>176</v>
+      </c>
+      <c r="J60" t="s">
+        <v>126</v>
+      </c>
+      <c r="K60" t="s">
+        <v>763</v>
+      </c>
+      <c r="L60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C61" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" t="s">
+        <v>173</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" t="s">
+        <v>149</v>
+      </c>
+      <c r="G61" t="s">
+        <v>592</v>
+      </c>
+      <c r="H61" t="s">
+        <v>1068</v>
+      </c>
+      <c r="I61" t="s">
+        <v>7</v>
+      </c>
+      <c r="J61" t="s">
+        <v>126</v>
+      </c>
+      <c r="K61" t="s">
+        <v>766</v>
+      </c>
+      <c r="L61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D62" t="s">
+        <v>173</v>
+      </c>
+      <c r="E62" t="s">
+        <v>28</v>
+      </c>
+      <c r="G62" t="s">
+        <v>1071</v>
+      </c>
+      <c r="H62" t="s">
+        <v>223</v>
+      </c>
+      <c r="I62" t="s">
+        <v>962</v>
+      </c>
+      <c r="J62" t="s">
+        <v>126</v>
+      </c>
+      <c r="K62" t="s">
+        <v>29</v>
+      </c>
+      <c r="L62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E63" t="s">
+        <v>1075</v>
+      </c>
+      <c r="F63" t="s">
+        <v>229</v>
+      </c>
+      <c r="G63" t="s">
+        <v>462</v>
+      </c>
+      <c r="H63" t="s">
+        <v>469</v>
+      </c>
+      <c r="I63" t="s">
+        <v>7</v>
+      </c>
+      <c r="J63" t="s">
+        <v>126</v>
+      </c>
+      <c r="K63" t="s">
+        <v>31</v>
+      </c>
+      <c r="L63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F64" t="s">
+        <v>229</v>
+      </c>
+      <c r="G64" t="s">
+        <v>462</v>
+      </c>
+      <c r="H64" t="s">
+        <v>161</v>
+      </c>
+      <c r="I64" t="s">
+        <v>7</v>
+      </c>
+      <c r="J64" t="s">
+        <v>126</v>
+      </c>
+      <c r="K64" t="s">
+        <v>1079</v>
+      </c>
+      <c r="L64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>181</v>
+      </c>
+      <c r="C65" t="s">
+        <v>182</v>
+      </c>
+      <c r="D65" t="s">
+        <v>173</v>
+      </c>
+      <c r="E65" t="s">
         <v>16</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F65" t="s">
         <v>183</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G65" t="s">
         <v>184</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H65" t="s">
         <v>143</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I65" t="s">
         <v>7</v>
       </c>
-      <c r="J21" t="s">
-        <v>126</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="J65" t="s">
+        <v>126</v>
+      </c>
+      <c r="K65" t="s">
         <v>17</v>
       </c>
-      <c r="L21" t="b">
+      <c r="L65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1074</v>
+      </c>
+      <c r="E66" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F66" t="s">
+        <v>229</v>
+      </c>
+      <c r="G66" t="s">
+        <v>462</v>
+      </c>
+      <c r="H66" t="s">
+        <v>161</v>
+      </c>
+      <c r="I66" t="s">
+        <v>7</v>
+      </c>
+      <c r="J66" t="s">
+        <v>126</v>
+      </c>
+      <c r="K66" t="s">
+        <v>1079</v>
+      </c>
+      <c r="L66" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N66" xr:uid="{772A3901-ADF4-4CA6-84A1-B1B329A6EAAE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3978,8 +5979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD6C127-FEDF-4C66-B64C-EEE91701B870}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView topLeftCell="E67" workbookViewId="0">
+      <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3996,6 +5997,7 @@
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -6199,7 +8201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>595</v>
       </c>
@@ -6234,7 +8236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>599</v>
       </c>
@@ -6269,7 +8271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>603</v>
       </c>
@@ -6301,7 +8303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>607</v>
       </c>
@@ -6336,7 +8338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>609</v>
       </c>
@@ -6371,7 +8373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>440</v>
       </c>
@@ -6406,7 +8408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>612</v>
       </c>
@@ -6441,7 +8443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>615</v>
       </c>
@@ -6476,7 +8478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>442</v>
       </c>
@@ -6511,7 +8513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>619</v>
       </c>
@@ -6546,7 +8548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>620</v>
       </c>
@@ -6581,7 +8583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>443</v>
       </c>
@@ -6616,7 +8618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>444</v>
       </c>
@@ -6651,7 +8653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>448</v>
       </c>
@@ -6686,7 +8688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>624</v>
       </c>
@@ -6721,7 +8723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>453</v>
       </c>
@@ -6755,8 +8757,14 @@
       <c r="L80" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M80" t="s">
+        <v>1084</v>
+      </c>
+      <c r="N80" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>628</v>
       </c>
@@ -6791,7 +8799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>178</v>
       </c>
@@ -6826,7 +8834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>629</v>
       </c>
@@ -6861,7 +8869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>470</v>
       </c>
@@ -6895,8 +8903,14 @@
       <c r="L84" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M84" t="s">
+        <v>1085</v>
+      </c>
+      <c r="N84" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>473</v>
       </c>
@@ -6930,8 +8944,14 @@
       <c r="L85" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M85" t="s">
+        <v>1085</v>
+      </c>
+      <c r="N85" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>634</v>
       </c>
@@ -6966,7 +8986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>476</v>
       </c>
@@ -7001,7 +9021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>639</v>
       </c>
@@ -7036,7 +9056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>644</v>
       </c>
@@ -7071,7 +9091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>648</v>
       </c>
@@ -7107,6 +9127,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N90" xr:uid="{8FD6C127-FEDF-4C66-B64C-EEE91701B870}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7116,7 +9137,7 @@
   <dimension ref="A1:N81"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N1"/>
+      <selection activeCell="C1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9923,6 +11944,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N1" xr:uid="{4FD11507-890B-44C7-9C31-D3A58EA5E7EF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9932,7 +11954,7 @@
   <dimension ref="A1:N77"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N1"/>
+      <selection activeCell="C1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12623,6 +14645,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N1" xr:uid="{40595CBE-0474-41E3-AC67-369DAA4F82D6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12631,8 +14654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E3C7E3-F923-4F66-ADD1-3770840339D6}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12649,6 +14672,7 @@
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -12971,6 +14995,12 @@
       <c r="L9" t="b">
         <v>0</v>
       </c>
+      <c r="M9" t="s">
+        <v>1083</v>
+      </c>
+      <c r="N9" t="s">
+        <v>937</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -13568,6 +15598,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N26" xr:uid="{03E3C7E3-F923-4F66-ADD1-3770840339D6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13577,7 +15608,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13594,6 +15625,7 @@
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add User Guide modal and improve PDF export layout
</commit_message>
<xml_diff>
--- a/Class Cancellation App.xlsx
+++ b/Class Cancellation App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rebecca\Class Cancellation app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F3D269-0FD4-43FD-AAD0-0C6C8BF8706C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8C5215-2F6E-4D18-8E5D-D356055D4EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3435" uniqueCount="1089">
   <si>
     <t>Date</t>
   </si>
@@ -3304,6 +3304,15 @@
   </si>
   <si>
     <t>Oct 7. 2025; Oct 14, 2025; Oct 21, 2025</t>
+  </si>
+  <si>
+    <t>eed als</t>
+  </si>
+  <si>
+    <t>Sept 3, 2025; Sept 10, 2025</t>
+  </si>
+  <si>
+    <t>Credits have been issued for the Sept classes</t>
   </si>
 </sst>
 </file>
@@ -3662,7 +3671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772A3901-ADF4-4CA6-84A1-B1B329A6EAAE}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E16" workbookViewId="0">
       <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
@@ -3680,7 +3689,7 @@
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -5979,7 +5988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD6C127-FEDF-4C66-B64C-EEE91701B870}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView topLeftCell="E67" workbookViewId="0">
+    <sheetView topLeftCell="E58" workbookViewId="0">
       <selection activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
@@ -9136,8 +9145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD11507-890B-44C7-9C31-D3A58EA5E7EF}">
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9154,6 +9163,7 @@
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -9710,7 +9720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>672</v>
       </c>
@@ -9745,7 +9755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>676</v>
       </c>
@@ -9780,7 +9790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>680</v>
       </c>
@@ -9815,7 +9825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>682</v>
       </c>
@@ -9850,7 +9860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>686</v>
       </c>
@@ -9885,7 +9895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>687</v>
       </c>
@@ -9920,7 +9930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>278</v>
       </c>
@@ -9954,8 +9964,14 @@
       <c r="L23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>1087</v>
+      </c>
+      <c r="N23" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>280</v>
       </c>
@@ -9987,7 +10003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>689</v>
       </c>
@@ -10022,7 +10038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>691</v>
       </c>
@@ -10054,7 +10070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>694</v>
       </c>
@@ -10089,7 +10105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>284</v>
       </c>
@@ -10124,7 +10140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>695</v>
       </c>
@@ -10159,7 +10175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>696</v>
       </c>
@@ -10191,7 +10207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>697</v>
       </c>
@@ -10223,7 +10239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>698</v>
       </c>
@@ -11953,7 +11969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40595CBE-0474-41E3-AC67-369DAA4F82D6}">
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C7" workbookViewId="0">
       <selection activeCell="C1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -14654,8 +14670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E3C7E3-F923-4F66-ADD1-3770840339D6}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14724,7 +14740,7 @@
         <v>250</v>
       </c>
       <c r="C2" t="s">
-        <v>251</v>
+        <v>1086</v>
       </c>
       <c r="D2" t="s">
         <v>252</v>

</xml_diff>

<commit_message>
Add sticky header and favorite star functionality
</commit_message>
<xml_diff>
--- a/Class Cancellation App.xlsx
+++ b/Class Cancellation App.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rebecca\Class Cancellation app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8C5215-2F6E-4D18-8E5D-D356055D4EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990739FE-010B-4DED-9C26-9FF4B1B573CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="9" r:id="rId1"/>
@@ -24,9 +24,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Friday!$A$1:$N$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Monday!$A$1:$N$66</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Thursday!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Thursday!$A$1:$N$77</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tuesday!$A$1:$N$90</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Wednesday!$A$1:$N$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Wednesday!$A$1:$N$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3435" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3445" uniqueCount="1095">
   <si>
     <t>Date</t>
   </si>
@@ -3313,6 +3313,24 @@
   </si>
   <si>
     <t>Credits have been issued for the Sept classes</t>
+  </si>
+  <si>
+    <t>Make up class on Nov 20</t>
+  </si>
+  <si>
+    <t>Credits have been issued for Oct classes</t>
+  </si>
+  <si>
+    <t>Make up class for Oct 8 on Nov 19</t>
+  </si>
+  <si>
+    <t>Credit issued for Oct 8 class on Sept 8</t>
+  </si>
+  <si>
+    <t>Make up class for Sept 18 on Nov 20</t>
+  </si>
+  <si>
+    <t>No makeup class set up for Sept 19 yet</t>
   </si>
 </sst>
 </file>
@@ -3672,7 +3690,7 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5988,8 +6006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD6C127-FEDF-4C66-B64C-EEE91701B870}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView topLeftCell="E58" workbookViewId="0">
-      <selection activeCell="J95" sqref="J95"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M102" sqref="M102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6007,6 +6025,7 @@
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
     <col min="13" max="13" width="35.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7120,7 +7139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>133</v>
       </c>
@@ -7155,7 +7174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>218</v>
       </c>
@@ -7190,7 +7209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>221</v>
       </c>
@@ -7222,7 +7241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>558</v>
       </c>
@@ -7254,7 +7273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>560</v>
       </c>
@@ -7286,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>562</v>
       </c>
@@ -7321,7 +7340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>564</v>
       </c>
@@ -7356,7 +7375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>225</v>
       </c>
@@ -7391,7 +7410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>227</v>
       </c>
@@ -7426,7 +7445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>232</v>
       </c>
@@ -7455,7 +7474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>235</v>
       </c>
@@ -7489,8 +7508,14 @@
       <c r="L43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M43" s="3">
+        <v>45916</v>
+      </c>
+      <c r="N43" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>239</v>
       </c>
@@ -7525,7 +7550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>565</v>
       </c>
@@ -7554,7 +7579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>567</v>
       </c>
@@ -7589,7 +7614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>242</v>
       </c>
@@ -7624,7 +7649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>246</v>
       </c>
@@ -8770,7 +8795,7 @@
         <v>1084</v>
       </c>
       <c r="N80" t="s">
-        <v>937</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
@@ -8916,7 +8941,7 @@
         <v>1085</v>
       </c>
       <c r="N84" t="s">
-        <v>937</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.25">
@@ -8957,7 +8982,7 @@
         <v>1085</v>
       </c>
       <c r="N85" t="s">
-        <v>937</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.25">
@@ -9145,16 +9170,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD11507-890B-44C7-9C31-D3A58EA5E7EF}">
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M88" sqref="M88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -9164,6 +9189,7 @@
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
     <col min="13" max="13" width="25.140625" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -9719,6 +9745,12 @@
       <c r="L16" t="b">
         <v>0</v>
       </c>
+      <c r="M16" s="3">
+        <v>45938</v>
+      </c>
+      <c r="N16" t="s">
+        <v>1091</v>
+      </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -10271,7 +10303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>699</v>
       </c>
@@ -10306,7 +10338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>700</v>
       </c>
@@ -10341,7 +10373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>144</v>
       </c>
@@ -10376,7 +10408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>702</v>
       </c>
@@ -10411,7 +10443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>148</v>
       </c>
@@ -10445,8 +10477,14 @@
       <c r="L37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="3">
+        <v>45938</v>
+      </c>
+      <c r="N37" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>287</v>
       </c>
@@ -10481,7 +10519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>292</v>
       </c>
@@ -10513,7 +10551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>295</v>
       </c>
@@ -10548,7 +10586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>706</v>
       </c>
@@ -10583,7 +10621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>707</v>
       </c>
@@ -10618,7 +10656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>300</v>
       </c>
@@ -10653,7 +10691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>304</v>
       </c>
@@ -10688,7 +10726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>710</v>
       </c>
@@ -10723,7 +10761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>712</v>
       </c>
@@ -10758,7 +10796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>153</v>
       </c>
@@ -10792,8 +10830,14 @@
       <c r="L47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M47" s="3">
+        <v>45938</v>
+      </c>
+      <c r="N47" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>154</v>
       </c>
@@ -10823,6 +10867,12 @@
       </c>
       <c r="L48" t="b">
         <v>0</v>
+      </c>
+      <c r="M48" s="3">
+        <v>45938</v>
+      </c>
+      <c r="N48" t="s">
+        <v>1092</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
@@ -11379,7 +11429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>739</v>
       </c>
@@ -11411,7 +11461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>328</v>
       </c>
@@ -11446,7 +11496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>330</v>
       </c>
@@ -11481,7 +11531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>155</v>
       </c>
@@ -11516,7 +11566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>742</v>
       </c>
@@ -11550,8 +11600,14 @@
       <c r="L69" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M69" s="3">
+        <v>45938</v>
+      </c>
+      <c r="N69" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>744</v>
       </c>
@@ -11586,7 +11642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>334</v>
       </c>
@@ -11618,7 +11674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>748</v>
       </c>
@@ -11650,7 +11706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>750</v>
       </c>
@@ -11682,7 +11738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>751</v>
       </c>
@@ -11717,7 +11773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>754</v>
       </c>
@@ -11752,7 +11808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>338</v>
       </c>
@@ -11787,7 +11843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>757</v>
       </c>
@@ -11822,7 +11878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>760</v>
       </c>
@@ -11857,7 +11913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>764</v>
       </c>
@@ -11892,7 +11948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>767</v>
       </c>
@@ -11960,7 +12016,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{4FD11507-890B-44C7-9C31-D3A58EA5E7EF}"/>
+  <autoFilter ref="A1:N81" xr:uid="{4FD11507-890B-44C7-9C31-D3A58EA5E7EF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11969,8 +12025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40595CBE-0474-41E3-AC67-369DAA4F82D6}">
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11987,6 +12043,8 @@
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="23.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -12082,7 +12140,7 @@
         <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>193</v>
+        <v>163</v>
       </c>
       <c r="G3" t="s">
         <v>216</v>
@@ -12376,6 +12434,12 @@
       <c r="L11" t="b">
         <v>0</v>
       </c>
+      <c r="M11" s="3">
+        <v>45918</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1093</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -12552,7 +12616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>357</v>
       </c>
@@ -12587,7 +12651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>783</v>
       </c>
@@ -12622,7 +12686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>784</v>
       </c>
@@ -12657,7 +12721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>786</v>
       </c>
@@ -12692,7 +12756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>790</v>
       </c>
@@ -12724,7 +12788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>793</v>
       </c>
@@ -12756,7 +12820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>361</v>
       </c>
@@ -12791,7 +12855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>796</v>
       </c>
@@ -12823,7 +12887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>797</v>
       </c>
@@ -12855,7 +12919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>798</v>
       </c>
@@ -12890,7 +12954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>800</v>
       </c>
@@ -12925,7 +12989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>801</v>
       </c>
@@ -12959,8 +13023,14 @@
       <c r="L28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="3">
+        <v>45918</v>
+      </c>
+      <c r="N28" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>367</v>
       </c>
@@ -12995,7 +13065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>369</v>
       </c>
@@ -13030,7 +13100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>162</v>
       </c>
@@ -13044,7 +13114,7 @@
         <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="G31" t="s">
         <v>124</v>
@@ -13065,7 +13135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>806</v>
       </c>
@@ -13654,7 +13724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>832</v>
       </c>
@@ -13689,7 +13759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>835</v>
       </c>
@@ -13723,8 +13793,14 @@
       <c r="L50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M50" s="3">
+        <v>45918</v>
+      </c>
+      <c r="N50" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>837</v>
       </c>
@@ -13759,7 +13835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>839</v>
       </c>
@@ -13794,7 +13870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>391</v>
       </c>
@@ -13829,7 +13905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>165</v>
       </c>
@@ -13864,7 +13940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>842</v>
       </c>
@@ -13899,7 +13975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>393</v>
       </c>
@@ -13931,7 +14007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>397</v>
       </c>
@@ -13966,7 +14042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>847</v>
       </c>
@@ -14001,7 +14077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>850</v>
       </c>
@@ -14033,7 +14109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>852</v>
       </c>
@@ -14067,8 +14143,14 @@
       <c r="L60" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M60" s="3">
+        <v>45918</v>
+      </c>
+      <c r="N60" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>855</v>
       </c>
@@ -14103,7 +14185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>856</v>
       </c>
@@ -14138,7 +14220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>860</v>
       </c>
@@ -14173,7 +14255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>862</v>
       </c>
@@ -14661,7 +14743,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N1" xr:uid="{40595CBE-0474-41E3-AC67-369DAA4F82D6}"/>
+  <autoFilter ref="A1:N77" xr:uid="{40595CBE-0474-41E3-AC67-369DAA4F82D6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Convert show all/cancellations buttons to dropdown filter for consistency
</commit_message>
<xml_diff>
--- a/Class Cancellation App.xlsx
+++ b/Class Cancellation App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rebecca\Class Cancellation app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990739FE-010B-4DED-9C26-9FF4B1B573CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285F9BA3-6B5E-41F7-92D8-AAB829C77BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="9" r:id="rId1"/>
@@ -6006,7 +6006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD6C127-FEDF-4C66-B64C-EEE91701B870}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="M102" sqref="M102"/>
     </sheetView>
   </sheetViews>
@@ -14752,8 +14752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E3C7E3-F923-4F66-ADD1-3770840339D6}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15238,6 +15238,9 @@
       </c>
       <c r="L13" t="b">
         <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>45912</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix date parsing issue: normalize periods to commas for better date display on mobile
</commit_message>
<xml_diff>
--- a/Class Cancellation App.xlsx
+++ b/Class Cancellation App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rebecca\Class Cancellation app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D6F6D9-F098-4311-A6D3-ECCCAA5A6D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F951433F-8CB7-4C8F-813A-C4462A5F1885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3445" uniqueCount="1095">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3445" uniqueCount="1094">
   <si>
     <t>Date</t>
   </si>
@@ -3301,9 +3301,6 @@
   </si>
   <si>
     <t>Oct 7, 2025; Oct 14, 2025; Oct 21, 2025</t>
-  </si>
-  <si>
-    <t>Oct 7. 2025; Oct 14, 2025; Oct 21, 2025</t>
   </si>
   <si>
     <t>eed als</t>
@@ -3689,7 +3686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772A3901-ADF4-4CA6-84A1-B1B329A6EAAE}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="E16" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
@@ -6006,8 +6003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD6C127-FEDF-4C66-B64C-EEE91701B870}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M102" sqref="M102"/>
+    <sheetView tabSelected="1" topLeftCell="E58" workbookViewId="0">
+      <selection activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7512,7 +7509,7 @@
         <v>45916</v>
       </c>
       <c r="N43" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
@@ -8795,7 +8792,7 @@
         <v>1084</v>
       </c>
       <c r="N80" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="81" spans="2:14" x14ac:dyDescent="0.25">
@@ -8938,10 +8935,10 @@
         <v>0</v>
       </c>
       <c r="M84" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="N84" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="85" spans="2:14" x14ac:dyDescent="0.25">
@@ -8979,10 +8976,10 @@
         <v>0</v>
       </c>
       <c r="M85" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="N85" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="86" spans="2:14" x14ac:dyDescent="0.25">
@@ -9749,7 +9746,7 @@
         <v>45938</v>
       </c>
       <c r="N16" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
@@ -9997,10 +9994,10 @@
         <v>0</v>
       </c>
       <c r="M23" t="s">
+        <v>1086</v>
+      </c>
+      <c r="N23" t="s">
         <v>1087</v>
-      </c>
-      <c r="N23" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
@@ -10481,7 +10478,7 @@
         <v>45938</v>
       </c>
       <c r="N37" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
@@ -10834,7 +10831,7 @@
         <v>45938</v>
       </c>
       <c r="N47" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
@@ -10872,7 +10869,7 @@
         <v>45938</v>
       </c>
       <c r="N48" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
@@ -11604,7 +11601,7 @@
         <v>45938</v>
       </c>
       <c r="N69" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.25">
@@ -12438,7 +12435,7 @@
         <v>45918</v>
       </c>
       <c r="N11" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -13027,7 +13024,7 @@
         <v>45918</v>
       </c>
       <c r="N28" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
@@ -13797,7 +13794,7 @@
         <v>45918</v>
       </c>
       <c r="N50" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
@@ -14147,7 +14144,7 @@
         <v>45918</v>
       </c>
       <c r="N60" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
@@ -14752,8 +14749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E3C7E3-F923-4F66-ADD1-3770840339D6}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14822,7 +14819,7 @@
         <v>250</v>
       </c>
       <c r="C2" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D2" t="s">
         <v>252</v>
@@ -15709,7 +15706,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove duplicate Add to Home Screen button from mobile controls section
</commit_message>
<xml_diff>
--- a/Class Cancellation App.xlsx
+++ b/Class Cancellation App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rebecca\Class Cancellation app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F951433F-8CB7-4C8F-813A-C4462A5F1885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5051C33-EFC8-460D-A0D7-EACF48C225A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3445" uniqueCount="1094">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3441" uniqueCount="1094">
   <si>
     <t>Date</t>
   </si>
@@ -6003,7 +6003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FD6C127-FEDF-4C66-B64C-EEE91701B870}">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E58" workbookViewId="0">
+    <sheetView topLeftCell="E58" workbookViewId="0">
       <selection activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
@@ -8795,7 +8795,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>628</v>
       </c>
@@ -8830,7 +8830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>178</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>629</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>470</v>
       </c>
@@ -8934,14 +8934,8 @@
       <c r="L84" t="b">
         <v>0</v>
       </c>
-      <c r="M84" t="s">
-        <v>1084</v>
-      </c>
-      <c r="N84" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>473</v>
       </c>
@@ -8975,14 +8969,8 @@
       <c r="L85" t="b">
         <v>0</v>
       </c>
-      <c r="M85" t="s">
-        <v>1084</v>
-      </c>
-      <c r="N85" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>634</v>
       </c>
@@ -9017,7 +9005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>476</v>
       </c>
@@ -9052,7 +9040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>639</v>
       </c>
@@ -9087,7 +9075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>644</v>
       </c>
@@ -9122,7 +9110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>648</v>
       </c>
@@ -14749,8 +14737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E3C7E3-F923-4F66-ADD1-3770840339D6}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Clean up unused imports and fix ESLint warnings to improve build performance
</commit_message>
<xml_diff>
--- a/Class Cancellation App.xlsx
+++ b/Class Cancellation App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rebecca\Class Cancellation app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5051C33-EFC8-460D-A0D7-EACF48C225A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EB994C-539C-4489-BACE-2FC95B2CA4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3441" uniqueCount="1094">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3443" uniqueCount="1096">
   <si>
     <t>Date</t>
   </si>
@@ -3328,6 +3328,12 @@
   </si>
   <si>
     <t>No makeup class set up for Sept 19 yet</t>
+  </si>
+  <si>
+    <t>TURE</t>
+  </si>
+  <si>
+    <t>Make up clss on for Sept 22 on Nov 17</t>
   </si>
 </sst>
 </file>
@@ -3375,11 +3381,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3686,8 +3695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772A3901-ADF4-4CA6-84A1-B1B329A6EAAE}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4815,7 +4824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>996</v>
       </c>
@@ -4850,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>998</v>
       </c>
@@ -4885,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>1001</v>
       </c>
@@ -4920,7 +4929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>1004</v>
       </c>
@@ -4955,7 +4964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>1007</v>
       </c>
@@ -4990,7 +4999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>1010</v>
       </c>
@@ -5025,7 +5034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>177</v>
       </c>
@@ -5060,7 +5069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>1011</v>
       </c>
@@ -5095,7 +5104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>1015</v>
       </c>
@@ -5127,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>1017</v>
       </c>
@@ -5159,7 +5168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>1018</v>
       </c>
@@ -5197,7 +5206,7 @@
         <v>45971</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>1022</v>
       </c>
@@ -5232,7 +5241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>1023</v>
       </c>
@@ -5267,7 +5276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>1027</v>
       </c>
@@ -5302,7 +5311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>1029</v>
       </c>
@@ -5334,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>1031</v>
       </c>
@@ -5367,6 +5376,12 @@
       </c>
       <c r="L48" t="b">
         <v>0</v>
+      </c>
+      <c r="M48" s="3">
+        <v>45922</v>
+      </c>
+      <c r="N48" t="s">
+        <v>1095</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
@@ -14737,8 +14752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E3C7E3-F923-4F66-ADD1-3770840339D6}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15539,8 +15554,8 @@
       <c r="K22" t="s">
         <v>921</v>
       </c>
-      <c r="L22" t="b">
-        <v>0</v>
+      <c r="L22" s="4" t="s">
+        <v>1094</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add comprehensive event list with improved scraping - All Seniors Kingston events for Oct-Dec 2025
</commit_message>
<xml_diff>
--- a/Class Cancellation App.xlsx
+++ b/Class Cancellation App.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rebecca\Class Cancellation app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EB994C-539C-4489-BACE-2FC95B2CA4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA6E170-4D9F-44D4-83B4-55539946D340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3333,7 +3333,7 @@
     <t>TURE</t>
   </si>
   <si>
-    <t>Make up clss on for Sept 22 on Nov 17</t>
+    <t>Make up class for Sept 22 on Nov 17</t>
   </si>
 </sst>
 </file>
@@ -3696,7 +3696,7 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix all tooltip issues: make bigger tooltips, position QR code to left, fix mobile visibility, add calendar navigation tooltips
</commit_message>
<xml_diff>
--- a/Class Cancellation App.xlsx
+++ b/Class Cancellation App.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Rebecca\Class Cancellation app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88588DC8-6DD5-4CDF-A4D4-CAF0F46CE9BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A15E1D-62CA-4EC1-8902-6251F7284CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="9" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3443" uniqueCount="1096">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3444" uniqueCount="1097">
   <si>
     <t>Date</t>
   </si>
@@ -3334,6 +3334,9 @@
   </si>
   <si>
     <t>Make up class for Sept 22 on Nov 17</t>
+  </si>
+  <si>
+    <t>Make up class for Sept 26 on Nov 21</t>
   </si>
 </sst>
 </file>
@@ -3695,7 +3698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772A3901-ADF4-4CA6-84A1-B1B329A6EAAE}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+    <sheetView topLeftCell="E19" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -14752,8 +14755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E3C7E3-F923-4F66-ADD1-3770840339D6}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15311,6 +15314,12 @@
       </c>
       <c r="L15" t="b">
         <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>45926</v>
+      </c>
+      <c r="N15" t="s">
+        <v>1096</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>